<commit_message>
PowerPoint and repo cleanup
</commit_message>
<xml_diff>
--- a/Machine_Learning/Optimization Summary.xlsx
+++ b/Machine_Learning/Optimization Summary.xlsx
@@ -60,9 +60,6 @@
     <t>class_weight='balanced', criterion='entropy', max_depth=150, max_leaf_nodes=32, min_samples_leaf=6, min_samples_split=4, n_estimators=800</t>
   </si>
   <si>
-    <t>class_weight='balanced', criterion='entropy', max_depth=150, max_depth=50, max_leaf_nodes=16, min_samples_leaf=6, min_samples_split=4, n_estimators=200</t>
-  </si>
-  <si>
     <t>n_neighbors=5, cutoff=5 min</t>
   </si>
   <si>
@@ -75,7 +72,10 @@
     <t>SVM</t>
   </si>
   <si>
-    <t>Incomplete after 1300 minutes</t>
+    <t>Incomplete after 1200+ minutes</t>
+  </si>
+  <si>
+    <t>class_weight='balanced', criterion='entropy', max_depth=50, max_leaf_nodes=16, min_samples_leaf=6, min_samples_split=4, n_estimators=200</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -630,12 +630,12 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -647,7 +647,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>